<commit_message>
Update the results description.
</commit_message>
<xml_diff>
--- a/src/mibench/BFWindow_Results.xlsx
+++ b/src/mibench/BFWindow_Results.xlsx
@@ -1114,11 +1114,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="168198912"/>
-        <c:axId val="168200448"/>
+        <c:axId val="164127488"/>
+        <c:axId val="164129024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168198912"/>
+        <c:axId val="164127488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,7 +1135,7 @@
             <a:tailEnd type="triangle" w="med" len="med"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="168200448"/>
+        <c:crossAx val="164129024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1143,7 +1143,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168200448"/>
+        <c:axId val="164129024"/>
         <c:scaling>
           <c:logBase val="1000"/>
           <c:orientation val="minMax"/>
@@ -1170,7 +1170,7 @@
             <a:tailEnd type="triangle" w="med" len="med"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="168198912"/>
+        <c:crossAx val="164127488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1824,11 +1824,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="168070528"/>
-        <c:axId val="168092800"/>
+        <c:axId val="165776768"/>
+        <c:axId val="165799040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168070528"/>
+        <c:axId val="165776768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1846,7 +1846,7 @@
             <a:tailEnd type="triangle"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="168092800"/>
+        <c:crossAx val="165799040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1855,7 +1855,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168092800"/>
+        <c:axId val="165799040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1880,7 +1880,7 @@
             <a:tailEnd type="triangle"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="168070528"/>
+        <c:crossAx val="165776768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1934,16 +1934,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>8964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>46808</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>297820</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>176604</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1966,16 +1966,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>8964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>54428</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>175259</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>305440</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>4929</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4311,10 +4311,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>